<commit_message>
Updates to incorporate pre-fire canopy cover analysis, and some code cleaning.
</commit_message>
<xml_diff>
--- a/Data/Raw/tc plot characteristics.xlsx
+++ b/Data/Raw/tc plot characteristics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/Berkeley/Post-Doc UCB/Research Projects/Side Projects/CO Thermophilization/co_thermo/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFD8086-6FF9-9942-B444-EDD62AFA898F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869695E9-1C47-964A-A498-E57F2D3A2646}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7680" yWindow="460" windowWidth="27740" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="196">
   <si>
     <t>plotyear</t>
   </si>
@@ -607,6 +607,12 @@
   </si>
   <si>
     <t>Slope</t>
+  </si>
+  <si>
+    <t>CanCovlive</t>
+  </si>
+  <si>
+    <t>CanCovlivedead</t>
   </si>
 </sst>
 </file>
@@ -977,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y141"/>
+  <dimension ref="A1:AA141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -991,10 +997,12 @@
     <col min="5" max="13" width="11.1640625" style="9" customWidth="1"/>
     <col min="14" max="14" width="11.1640625" style="5" customWidth="1"/>
     <col min="15" max="25" width="11.1640625" style="9" customWidth="1"/>
-    <col min="26" max="16384" width="9.1640625" style="9"/>
+    <col min="26" max="26" width="9.1640625" style="9"/>
+    <col min="27" max="27" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1070,8 +1078,14 @@
       <c r="Y1" s="9" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z1" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1147,8 +1161,15 @@
       <c r="Y2" s="9">
         <v>22.768999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z2" s="9">
+        <f>30.715*LN(Y2) - 36.502</f>
+        <v>59.494659822879179</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>66.711930016063462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1225,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1302,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1379,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1456,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1533,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -1610,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -1686,8 +1707,15 @@
       <c r="Y9" s="9">
         <v>10.5739</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z9" s="9">
+        <f>30.715*LN(Y9) - 36.502</f>
+        <v>35.935908939219864</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>39.175252284727016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
@@ -1764,7 +1792,7 @@
         <v>12.1173</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>69</v>
       </c>
@@ -1841,7 +1869,7 @@
         <v>12.316199999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>79</v>
       </c>
@@ -1918,7 +1946,7 @@
         <v>12.525399999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>89</v>
       </c>
@@ -1995,7 +2023,7 @@
         <v>12.737300000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>99</v>
       </c>
@@ -2072,7 +2100,7 @@
         <v>12.9518</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>109</v>
       </c>
@@ -2149,7 +2177,7 @@
         <v>14.060699999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
@@ -2225,8 +2253,15 @@
       <c r="Y16" s="9">
         <v>17.829999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z16" s="9">
+        <f>30.715*LN(Y16) - 36.502</f>
+        <v>51.984303895042125</v>
+      </c>
+      <c r="AA16" s="9">
+        <v>58.46727899771161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>60</v>
       </c>
@@ -2303,7 +2338,7 @@
         <v>18.4283</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>70</v>
       </c>
@@ -2380,7 +2415,7 @@
         <v>18.494999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>80</v>
       </c>
@@ -2457,7 +2492,7 @@
         <v>18.595700000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>90</v>
       </c>
@@ -2534,7 +2569,7 @@
         <v>18.748900000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>100</v>
       </c>
@@ -2611,7 +2646,7 @@
         <v>18.909199999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>110</v>
       </c>
@@ -2688,7 +2723,7 @@
         <v>19.3932</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -2764,8 +2799,15 @@
       <c r="Y23" s="9">
         <v>14.7698</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z23" s="9">
+        <f>30.715*LN(Y23) - 36.502</f>
+        <v>46.200734621881502</v>
+      </c>
+      <c r="AA23" s="9">
+        <v>43.416853405796992</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -2842,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -2919,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -2996,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -3073,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
@@ -3150,7 +3192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -3227,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
@@ -3303,8 +3345,15 @@
       <c r="Y30" s="9">
         <v>18.0092</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z30" s="9">
+        <f>30.715*LN(Y30) - 36.502</f>
+        <v>52.2914633110151</v>
+      </c>
+      <c r="AA30" s="9">
+        <v>54.592190619411916</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
@@ -3381,7 +3430,7 @@
         <v>15.1471</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>71</v>
       </c>
@@ -3458,7 +3507,7 @@
         <v>11.718</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>81</v>
       </c>
@@ -3535,7 +3584,7 @@
         <v>11.852399999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>91</v>
       </c>
@@ -3612,7 +3661,7 @@
         <v>10.308900000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>101</v>
       </c>
@@ -3689,7 +3738,7 @@
         <v>10.437899999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>111</v>
       </c>
@@ -3766,7 +3815,7 @@
         <v>11.1412</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -3842,8 +3891,15 @@
       <c r="Y37" s="9">
         <v>20.133600000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z37" s="9">
+        <f>30.715*LN(Y37) - 36.502</f>
+        <v>55.716410730312624</v>
+      </c>
+      <c r="AA37" s="9">
+        <v>58.215170879177968</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>62</v>
       </c>
@@ -3920,7 +3976,7 @@
         <v>16.6221</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
@@ -3997,7 +4053,7 @@
         <v>16.414400000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
@@ -4074,7 +4130,7 @@
         <v>16.401800000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>92</v>
       </c>
@@ -4151,7 +4207,7 @@
         <v>15.003599999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>102</v>
       </c>
@@ -4228,7 +4284,7 @@
         <v>15.061600000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>112</v>
       </c>
@@ -4305,7 +4361,7 @@
         <v>14.994300000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>119</v>
       </c>
@@ -4381,8 +4437,15 @@
       <c r="Y44" s="9">
         <v>16.9635</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z44" s="9">
+        <f>30.715*LN(Y44) - 36.502</f>
+        <v>50.45413005347374</v>
+      </c>
+      <c r="AA44" s="9">
+        <v>53.660387990080217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>132</v>
       </c>
@@ -4459,7 +4522,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>138</v>
       </c>
@@ -4536,7 +4599,7 @@
         <v>6.8396999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>144</v>
       </c>
@@ -4613,7 +4676,7 @@
         <v>6.0465</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>150</v>
       </c>
@@ -4690,7 +4753,7 @@
         <v>5.7102999999999993</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>156</v>
       </c>
@@ -4767,7 +4830,7 @@
         <v>5.7963999999999993</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>162</v>
       </c>
@@ -4844,7 +4907,7 @@
         <v>6.2353000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>47</v>
       </c>
@@ -4920,8 +4983,15 @@
       <c r="Y51" s="9">
         <v>12.880099999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z51" s="9">
+        <f>30.715*LN(Y51) - 36.502</f>
+        <v>41.995818230140877</v>
+      </c>
+      <c r="AA51" s="9">
+        <v>45.866606724298499</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>63</v>
       </c>
@@ -4998,7 +5068,7 @@
         <v>13.684699999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>73</v>
       </c>
@@ -5075,7 +5145,7 @@
         <v>13.804599999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>83</v>
       </c>
@@ -5152,7 +5222,7 @@
         <v>13.934699999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>93</v>
       </c>
@@ -5229,7 +5299,7 @@
         <v>14.066399999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>103</v>
       </c>
@@ -5306,7 +5376,7 @@
         <v>14.199900000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>113</v>
       </c>
@@ -5383,7 +5453,7 @@
         <v>11.311199999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>122</v>
       </c>
@@ -5459,8 +5529,15 @@
       <c r="Y58" s="9">
         <v>18.5183</v>
       </c>
-    </row>
-    <row r="59" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z58" s="9">
+        <f>30.715*LN(Y58) - 36.502</f>
+        <v>53.147695964576251</v>
+      </c>
+      <c r="AA58" s="9">
+        <v>53.332408365403559</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>133</v>
       </c>
@@ -5537,7 +5614,7 @@
         <v>7.3336999999999994</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>139</v>
       </c>
@@ -5614,7 +5691,7 @@
         <v>7.0853000000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>145</v>
       </c>
@@ -5691,7 +5768,7 @@
         <v>5.6995000000000005</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>151</v>
       </c>
@@ -5768,7 +5845,7 @@
         <v>5.6292</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>157</v>
       </c>
@@ -5845,7 +5922,7 @@
         <v>5.5898000000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>163</v>
       </c>
@@ -5922,7 +5999,7 @@
         <v>4.1969000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>124</v>
       </c>
@@ -5998,8 +6075,15 @@
       <c r="Y65" s="9">
         <v>20.4283</v>
       </c>
-    </row>
-    <row r="66" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z65" s="9">
+        <f>30.715*LN(Y65) - 36.502</f>
+        <v>56.162734486089313</v>
+      </c>
+      <c r="AA65" s="9">
+        <v>58.882914568715172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>134</v>
       </c>
@@ -6076,7 +6160,7 @@
         <v>16.859199999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>140</v>
       </c>
@@ -6153,7 +6237,7 @@
         <v>16.545400000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>146</v>
       </c>
@@ -6230,7 +6314,7 @@
         <v>16.631700000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>152</v>
       </c>
@@ -6307,7 +6391,7 @@
         <v>16.708000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>158</v>
       </c>
@@ -6384,7 +6468,7 @@
         <v>16.833500000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>164</v>
       </c>
@@ -6461,7 +6545,7 @@
         <v>17.388599999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>49</v>
       </c>
@@ -6537,8 +6621,15 @@
       <c r="Y72" s="9">
         <v>11.148100000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z72" s="9">
+        <f>30.715*LN(Y72) - 36.502</f>
+        <v>37.560129786006094</v>
+      </c>
+      <c r="AA72" s="9">
+        <v>41.563305229263513</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>64</v>
       </c>
@@ -6615,7 +6706,7 @@
         <v>11.566799999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>74</v>
       </c>
@@ -6692,7 +6783,7 @@
         <v>10.1983</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>84</v>
       </c>
@@ -6769,7 +6860,7 @@
         <v>10.347799999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>94</v>
       </c>
@@ -6846,7 +6937,7 @@
         <v>9.8882999999999992</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>104</v>
       </c>
@@ -6923,7 +7014,7 @@
         <v>6.5200000000000005</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>114</v>
       </c>
@@ -7000,7 +7091,7 @@
         <v>6.5036000000000005</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>51</v>
       </c>
@@ -7076,8 +7167,15 @@
       <c r="Y79" s="9">
         <v>15.608700000000002</v>
       </c>
-    </row>
-    <row r="80" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z79" s="9">
+        <f>30.715*LN(Y79) - 36.502</f>
+        <v>47.89755087586277</v>
+      </c>
+      <c r="AA79" s="9">
+        <v>48.48480297777089</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>65</v>
       </c>
@@ -7154,7 +7252,7 @@
         <v>13.0893</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>75</v>
       </c>
@@ -7231,7 +7329,7 @@
         <v>13.211499999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>85</v>
       </c>
@@ -7308,7 +7406,7 @@
         <v>13.3347</v>
       </c>
     </row>
-    <row r="83" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>95</v>
       </c>
@@ -7385,7 +7483,7 @@
         <v>13.4587</v>
       </c>
     </row>
-    <row r="84" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>105</v>
       </c>
@@ -7462,7 +7560,7 @@
         <v>13.1172</v>
       </c>
     </row>
-    <row r="85" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>115</v>
       </c>
@@ -7539,7 +7637,7 @@
         <v>13.661099999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>53</v>
       </c>
@@ -7615,8 +7713,15 @@
       <c r="Y86" s="9">
         <v>16.379300000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z86" s="9">
+        <f>30.715*LN(Y86) - 36.502</f>
+        <v>49.377703388935963</v>
+      </c>
+      <c r="AA86" s="9">
+        <v>51.410500057748628</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>66</v>
       </c>
@@ -7693,7 +7798,7 @@
         <v>17.383900000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>76</v>
       </c>
@@ -7770,7 +7875,7 @@
         <v>17.520400000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>86</v>
       </c>
@@ -7847,7 +7952,7 @@
         <v>17.658000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>96</v>
       </c>
@@ -7924,7 +8029,7 @@
         <v>17.796499999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>106</v>
       </c>
@@ -8001,7 +8106,7 @@
         <v>17.9361</v>
       </c>
     </row>
-    <row r="92" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>116</v>
       </c>
@@ -8078,7 +8183,7 @@
         <v>18.617899999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>126</v>
       </c>
@@ -8154,8 +8259,15 @@
       <c r="Y93" s="9">
         <v>19.531500000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z93" s="9">
+        <f>30.715*LN(Y93) - 36.502</f>
+        <v>54.783856816643812</v>
+      </c>
+      <c r="AA93" s="9">
+        <v>56.80505440362321</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>135</v>
       </c>
@@ -8232,7 +8344,7 @@
         <v>14.8566</v>
       </c>
     </row>
-    <row r="95" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>141</v>
       </c>
@@ -8309,7 +8421,7 @@
         <v>14.480399999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>147</v>
       </c>
@@ -8386,7 +8498,7 @@
         <v>14.5411</v>
       </c>
     </row>
-    <row r="97" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>153</v>
       </c>
@@ -8463,7 +8575,7 @@
         <v>14.280299999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>159</v>
       </c>
@@ -8540,7 +8652,7 @@
         <v>14.337799999999998</v>
       </c>
     </row>
-    <row r="99" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>165</v>
       </c>
@@ -8617,7 +8729,7 @@
         <v>14.5092</v>
       </c>
     </row>
-    <row r="100" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>128</v>
       </c>
@@ -8693,8 +8805,15 @@
       <c r="Y100" s="9">
         <v>18.040800000000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z100" s="9">
+        <f>30.715*LN(Y100) - 36.502</f>
+        <v>52.345310426054645</v>
+      </c>
+      <c r="AA100" s="9">
+        <v>58.979092236206519</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>136</v>
       </c>
@@ -8771,7 +8890,7 @@
         <v>7.5429999999999993</v>
       </c>
     </row>
-    <row r="102" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>142</v>
       </c>
@@ -8848,7 +8967,7 @@
         <v>5.1168999999999993</v>
       </c>
     </row>
-    <row r="103" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>148</v>
       </c>
@@ -8925,7 +9044,7 @@
         <v>4.3573000000000004</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>154</v>
       </c>
@@ -9002,7 +9121,7 @@
         <v>4.2392000000000003</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>160</v>
       </c>
@@ -9079,7 +9198,7 @@
         <v>3.4157000000000002</v>
       </c>
     </row>
-    <row r="106" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>166</v>
       </c>
@@ -9156,7 +9275,7 @@
         <v>2.2458</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>130</v>
       </c>
@@ -9232,8 +9351,15 @@
       <c r="Y107" s="9">
         <v>21.544999999999995</v>
       </c>
-    </row>
-    <row r="108" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z107" s="9">
+        <f>30.715*LN(Y107) - 36.502</f>
+        <v>57.797465928347499</v>
+      </c>
+      <c r="AA107" s="9">
+        <v>59.509495055554687</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>137</v>
       </c>
@@ -9310,7 +9436,7 @@
         <v>12.883700000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>143</v>
       </c>
@@ -9387,7 +9513,7 @@
         <v>11.504200000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>149</v>
       </c>
@@ -9464,7 +9590,7 @@
         <v>10.4701</v>
       </c>
     </row>
-    <row r="111" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>155</v>
       </c>
@@ -9541,7 +9667,7 @@
         <v>8.6364000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>161</v>
       </c>
@@ -9618,7 +9744,7 @@
         <v>8.7139000000000006</v>
       </c>
     </row>
-    <row r="113" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>167</v>
       </c>
@@ -9695,7 +9821,7 @@
         <v>9.1094999999999988</v>
       </c>
     </row>
-    <row r="114" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>10</v>
       </c>
@@ -9771,8 +9897,15 @@
       <c r="Y114" s="9">
         <v>16.821999999999999</v>
       </c>
-    </row>
-    <row r="115" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z114" s="9">
+        <f>30.715*LN(Y114) - 36.502</f>
+        <v>50.196848206988641</v>
+      </c>
+      <c r="AA114" s="9">
+        <v>55.999466701546275</v>
+      </c>
+    </row>
+    <row r="115" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>16</v>
       </c>
@@ -9849,7 +9982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>20</v>
       </c>
@@ -9926,7 +10059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>24</v>
       </c>
@@ -10003,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>28</v>
       </c>
@@ -10080,7 +10213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>32</v>
       </c>
@@ -10157,7 +10290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>36</v>
       </c>
@@ -10234,7 +10367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>55</v>
       </c>
@@ -10310,8 +10443,15 @@
       <c r="Y121" s="9">
         <v>15.588800000000001</v>
       </c>
-    </row>
-    <row r="122" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z121" s="9">
+        <f>30.715*LN(Y121) - 36.502</f>
+        <v>47.858366416665781</v>
+      </c>
+      <c r="AA121" s="9">
+        <v>52.104653895086663</v>
+      </c>
+    </row>
+    <row r="122" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>67</v>
       </c>
@@ -10388,7 +10528,7 @@
         <v>14.254100000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>77</v>
       </c>
@@ -10465,7 +10605,7 @@
         <v>13.208599999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>87</v>
       </c>
@@ -10542,7 +10682,7 @@
         <v>11.1829</v>
       </c>
     </row>
-    <row r="125" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>97</v>
       </c>
@@ -10619,7 +10759,7 @@
         <v>9.1695000000000011</v>
       </c>
     </row>
-    <row r="126" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>107</v>
       </c>
@@ -10696,7 +10836,7 @@
         <v>8.557599999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>117</v>
       </c>
@@ -10773,7 +10913,7 @@
         <v>8.8149999999999995</v>
       </c>
     </row>
-    <row r="128" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>57</v>
       </c>
@@ -10849,8 +10989,15 @@
       <c r="Y128" s="9">
         <v>19.6233</v>
       </c>
-    </row>
-    <row r="129" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z128" s="9">
+        <f>30.715*LN(Y128) - 36.502</f>
+        <v>54.927882180911205</v>
+      </c>
+      <c r="AA128" s="9">
+        <v>60.057395161179436</v>
+      </c>
+    </row>
+    <row r="129" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>68</v>
       </c>
@@ -10927,7 +11074,7 @@
         <v>19.708800000000004</v>
       </c>
     </row>
-    <row r="130" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>78</v>
       </c>
@@ -11004,7 +11151,7 @@
         <v>19.850200000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>88</v>
       </c>
@@ -11081,7 +11228,7 @@
         <v>19.947099999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>98</v>
       </c>
@@ -11158,7 +11305,7 @@
         <v>20.203799999999998</v>
       </c>
     </row>
-    <row r="133" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>108</v>
       </c>
@@ -11235,7 +11382,7 @@
         <v>20.465299999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>118</v>
       </c>
@@ -11312,7 +11459,7 @@
         <v>20.934400000000004</v>
       </c>
     </row>
-    <row r="135" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>12</v>
       </c>
@@ -11388,8 +11535,15 @@
       <c r="Y135" s="9">
         <v>14.170199999999999</v>
       </c>
-    </row>
-    <row r="136" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="Z135" s="9">
+        <f>30.715*LN(Y135) - 36.502</f>
+        <v>44.92780097293997</v>
+      </c>
+      <c r="AA135" s="9">
+        <v>44.970689041346482</v>
+      </c>
+    </row>
+    <row r="136" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>17</v>
       </c>
@@ -11466,7 +11620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>21</v>
       </c>
@@ -11543,7 +11697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>25</v>
       </c>
@@ -11620,7 +11774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>29</v>
       </c>
@@ -11697,7 +11851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>33</v>
       </c>
@@ -11774,7 +11928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>37</v>
       </c>
@@ -11852,10 +12006,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y141">
-    <sortCondition ref="B2:B141"/>
-    <sortCondition ref="C2:C141"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Additional updates in response to reviewer comments, plus formatting figures.
</commit_message>
<xml_diff>
--- a/Data/Raw/tc plot characteristics.xlsx
+++ b/Data/Raw/tc plot characteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/Berkeley/Post-Doc UCB/Research Projects/Side Projects/CO Thermophilization/co_thermo/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869695E9-1C47-964A-A498-E57F2D3A2646}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2709E1F7-70E1-9044-9FE6-C0296A30052A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="460" windowWidth="27740" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15620" yWindow="460" windowWidth="24860" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="197">
   <si>
     <t>plotyear</t>
   </si>
@@ -609,10 +609,13 @@
     <t>Slope</t>
   </si>
   <si>
-    <t>CanCovlive</t>
-  </si>
-  <si>
-    <t>CanCovlivedead</t>
+    <t>CanCovlive_regression</t>
+  </si>
+  <si>
+    <t>CanCovlivedead_regression</t>
+  </si>
+  <si>
+    <t>CanCovLive_FVS</t>
   </si>
 </sst>
 </file>
@@ -983,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA141"/>
+  <dimension ref="A1:AB141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1002,7 +1005,7 @@
     <col min="28" max="16384" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1084,8 +1087,11 @@
       <c r="AA1" s="5" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB1" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1168,8 +1174,11 @@
       <c r="AA2" s="9">
         <v>66.711930016063462</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB2" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1246,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1323,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1477,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1554,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -1631,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -1714,8 +1723,11 @@
       <c r="AA9" s="9">
         <v>39.175252284727016</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB9" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
@@ -1792,7 +1804,7 @@
         <v>12.1173</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>69</v>
       </c>
@@ -1869,7 +1881,7 @@
         <v>12.316199999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>79</v>
       </c>
@@ -1946,7 +1958,7 @@
         <v>12.525399999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>89</v>
       </c>
@@ -2023,7 +2035,7 @@
         <v>12.737300000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>99</v>
       </c>
@@ -2100,7 +2112,7 @@
         <v>12.9518</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>109</v>
       </c>
@@ -2177,7 +2189,7 @@
         <v>14.060699999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
@@ -2260,8 +2272,11 @@
       <c r="AA16" s="9">
         <v>58.46727899771161</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB16" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>60</v>
       </c>
@@ -2338,7 +2353,7 @@
         <v>18.4283</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>70</v>
       </c>
@@ -2415,7 +2430,7 @@
         <v>18.494999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>80</v>
       </c>
@@ -2492,7 +2507,7 @@
         <v>18.595700000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>90</v>
       </c>
@@ -2569,7 +2584,7 @@
         <v>18.748900000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>100</v>
       </c>
@@ -2646,7 +2661,7 @@
         <v>18.909199999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>110</v>
       </c>
@@ -2723,7 +2738,7 @@
         <v>19.3932</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -2806,8 +2821,11 @@
       <c r="AA23" s="9">
         <v>43.416853405796992</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB23" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -2884,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -2961,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -3038,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -3115,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
@@ -3192,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -3269,7 +3287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
@@ -3352,8 +3370,11 @@
       <c r="AA30" s="9">
         <v>54.592190619411916</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB30" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
@@ -3430,7 +3451,7 @@
         <v>15.1471</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>71</v>
       </c>
@@ -3507,7 +3528,7 @@
         <v>11.718</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>81</v>
       </c>
@@ -3584,7 +3605,7 @@
         <v>11.852399999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>91</v>
       </c>
@@ -3661,7 +3682,7 @@
         <v>10.308900000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>101</v>
       </c>
@@ -3738,7 +3759,7 @@
         <v>10.437899999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>111</v>
       </c>
@@ -3815,7 +3836,7 @@
         <v>11.1412</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -3898,8 +3919,11 @@
       <c r="AA37" s="9">
         <v>58.215170879177968</v>
       </c>
-    </row>
-    <row r="38" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB37" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>62</v>
       </c>
@@ -3976,7 +4000,7 @@
         <v>16.6221</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
@@ -4053,7 +4077,7 @@
         <v>16.414400000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
@@ -4130,7 +4154,7 @@
         <v>16.401800000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>92</v>
       </c>
@@ -4207,7 +4231,7 @@
         <v>15.003599999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>102</v>
       </c>
@@ -4284,7 +4308,7 @@
         <v>15.061600000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>112</v>
       </c>
@@ -4361,7 +4385,7 @@
         <v>14.994300000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>119</v>
       </c>
@@ -4444,8 +4468,11 @@
       <c r="AA44" s="9">
         <v>53.660387990080217</v>
       </c>
-    </row>
-    <row r="45" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB44" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>132</v>
       </c>
@@ -4522,7 +4549,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>138</v>
       </c>
@@ -4599,7 +4626,7 @@
         <v>6.8396999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>144</v>
       </c>
@@ -4676,7 +4703,7 @@
         <v>6.0465</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>150</v>
       </c>
@@ -4753,7 +4780,7 @@
         <v>5.7102999999999993</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>156</v>
       </c>
@@ -4830,7 +4857,7 @@
         <v>5.7963999999999993</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>162</v>
       </c>
@@ -4907,7 +4934,7 @@
         <v>6.2353000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>47</v>
       </c>
@@ -4990,8 +5017,11 @@
       <c r="AA51" s="9">
         <v>45.866606724298499</v>
       </c>
-    </row>
-    <row r="52" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB51" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>63</v>
       </c>
@@ -5068,7 +5098,7 @@
         <v>13.684699999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>73</v>
       </c>
@@ -5145,7 +5175,7 @@
         <v>13.804599999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>83</v>
       </c>
@@ -5222,7 +5252,7 @@
         <v>13.934699999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>93</v>
       </c>
@@ -5299,7 +5329,7 @@
         <v>14.066399999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>103</v>
       </c>
@@ -5376,7 +5406,7 @@
         <v>14.199900000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>113</v>
       </c>
@@ -5453,7 +5483,7 @@
         <v>11.311199999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>122</v>
       </c>
@@ -5536,8 +5566,11 @@
       <c r="AA58" s="9">
         <v>53.332408365403559</v>
       </c>
-    </row>
-    <row r="59" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB58" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>133</v>
       </c>
@@ -5614,7 +5647,7 @@
         <v>7.3336999999999994</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>139</v>
       </c>
@@ -5691,7 +5724,7 @@
         <v>7.0853000000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>145</v>
       </c>
@@ -5768,7 +5801,7 @@
         <v>5.6995000000000005</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>151</v>
       </c>
@@ -5845,7 +5878,7 @@
         <v>5.6292</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>157</v>
       </c>
@@ -5922,7 +5955,7 @@
         <v>5.5898000000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>163</v>
       </c>
@@ -5999,7 +6032,7 @@
         <v>4.1969000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>124</v>
       </c>
@@ -6082,8 +6115,11 @@
       <c r="AA65" s="9">
         <v>58.882914568715172</v>
       </c>
-    </row>
-    <row r="66" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB65" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>134</v>
       </c>
@@ -6160,7 +6196,7 @@
         <v>16.859199999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>140</v>
       </c>
@@ -6237,7 +6273,7 @@
         <v>16.545400000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>146</v>
       </c>
@@ -6314,7 +6350,7 @@
         <v>16.631700000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>152</v>
       </c>
@@ -6391,7 +6427,7 @@
         <v>16.708000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>158</v>
       </c>
@@ -6468,7 +6504,7 @@
         <v>16.833500000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>164</v>
       </c>
@@ -6545,7 +6581,7 @@
         <v>17.388599999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>49</v>
       </c>
@@ -6628,8 +6664,11 @@
       <c r="AA72" s="9">
         <v>41.563305229263513</v>
       </c>
-    </row>
-    <row r="73" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB72" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>64</v>
       </c>
@@ -6706,7 +6745,7 @@
         <v>11.566799999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>74</v>
       </c>
@@ -6783,7 +6822,7 @@
         <v>10.1983</v>
       </c>
     </row>
-    <row r="75" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>84</v>
       </c>
@@ -6860,7 +6899,7 @@
         <v>10.347799999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>94</v>
       </c>
@@ -6937,7 +6976,7 @@
         <v>9.8882999999999992</v>
       </c>
     </row>
-    <row r="77" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>104</v>
       </c>
@@ -7014,7 +7053,7 @@
         <v>6.5200000000000005</v>
       </c>
     </row>
-    <row r="78" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>114</v>
       </c>
@@ -7091,7 +7130,7 @@
         <v>6.5036000000000005</v>
       </c>
     </row>
-    <row r="79" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>51</v>
       </c>
@@ -7174,8 +7213,11 @@
       <c r="AA79" s="9">
         <v>48.48480297777089</v>
       </c>
-    </row>
-    <row r="80" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB79" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>65</v>
       </c>
@@ -7252,7 +7294,7 @@
         <v>13.0893</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>75</v>
       </c>
@@ -7329,7 +7371,7 @@
         <v>13.211499999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>85</v>
       </c>
@@ -7406,7 +7448,7 @@
         <v>13.3347</v>
       </c>
     </row>
-    <row r="83" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>95</v>
       </c>
@@ -7483,7 +7525,7 @@
         <v>13.4587</v>
       </c>
     </row>
-    <row r="84" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>105</v>
       </c>
@@ -7560,7 +7602,7 @@
         <v>13.1172</v>
       </c>
     </row>
-    <row r="85" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>115</v>
       </c>
@@ -7637,7 +7679,7 @@
         <v>13.661099999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>53</v>
       </c>
@@ -7720,8 +7762,11 @@
       <c r="AA86" s="9">
         <v>51.410500057748628</v>
       </c>
-    </row>
-    <row r="87" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB86" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>66</v>
       </c>
@@ -7798,7 +7843,7 @@
         <v>17.383900000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>76</v>
       </c>
@@ -7875,7 +7920,7 @@
         <v>17.520400000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>86</v>
       </c>
@@ -7952,7 +7997,7 @@
         <v>17.658000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>96</v>
       </c>
@@ -8029,7 +8074,7 @@
         <v>17.796499999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>106</v>
       </c>
@@ -8106,7 +8151,7 @@
         <v>17.9361</v>
       </c>
     </row>
-    <row r="92" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>116</v>
       </c>
@@ -8183,7 +8228,7 @@
         <v>18.617899999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>126</v>
       </c>
@@ -8266,8 +8311,11 @@
       <c r="AA93" s="9">
         <v>56.80505440362321</v>
       </c>
-    </row>
-    <row r="94" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB93" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>135</v>
       </c>
@@ -8344,7 +8392,7 @@
         <v>14.8566</v>
       </c>
     </row>
-    <row r="95" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>141</v>
       </c>
@@ -8421,7 +8469,7 @@
         <v>14.480399999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>147</v>
       </c>
@@ -8498,7 +8546,7 @@
         <v>14.5411</v>
       </c>
     </row>
-    <row r="97" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>153</v>
       </c>
@@ -8575,7 +8623,7 @@
         <v>14.280299999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>159</v>
       </c>
@@ -8652,7 +8700,7 @@
         <v>14.337799999999998</v>
       </c>
     </row>
-    <row r="99" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>165</v>
       </c>
@@ -8729,7 +8777,7 @@
         <v>14.5092</v>
       </c>
     </row>
-    <row r="100" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>128</v>
       </c>
@@ -8812,8 +8860,11 @@
       <c r="AA100" s="9">
         <v>58.979092236206519</v>
       </c>
-    </row>
-    <row r="101" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB100" s="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>136</v>
       </c>
@@ -8890,7 +8941,7 @@
         <v>7.5429999999999993</v>
       </c>
     </row>
-    <row r="102" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>142</v>
       </c>
@@ -8967,7 +9018,7 @@
         <v>5.1168999999999993</v>
       </c>
     </row>
-    <row r="103" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>148</v>
       </c>
@@ -9044,7 +9095,7 @@
         <v>4.3573000000000004</v>
       </c>
     </row>
-    <row r="104" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>154</v>
       </c>
@@ -9121,7 +9172,7 @@
         <v>4.2392000000000003</v>
       </c>
     </row>
-    <row r="105" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>160</v>
       </c>
@@ -9198,7 +9249,7 @@
         <v>3.4157000000000002</v>
       </c>
     </row>
-    <row r="106" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>166</v>
       </c>
@@ -9275,7 +9326,7 @@
         <v>2.2458</v>
       </c>
     </row>
-    <row r="107" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>130</v>
       </c>
@@ -9358,8 +9409,11 @@
       <c r="AA107" s="9">
         <v>59.509495055554687</v>
       </c>
-    </row>
-    <row r="108" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB107" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>137</v>
       </c>
@@ -9436,7 +9490,7 @@
         <v>12.883700000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>143</v>
       </c>
@@ -9513,7 +9567,7 @@
         <v>11.504200000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>149</v>
       </c>
@@ -9590,7 +9644,7 @@
         <v>10.4701</v>
       </c>
     </row>
-    <row r="111" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>155</v>
       </c>
@@ -9667,7 +9721,7 @@
         <v>8.6364000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>161</v>
       </c>
@@ -9744,7 +9798,7 @@
         <v>8.7139000000000006</v>
       </c>
     </row>
-    <row r="113" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>167</v>
       </c>
@@ -9821,7 +9875,7 @@
         <v>9.1094999999999988</v>
       </c>
     </row>
-    <row r="114" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>10</v>
       </c>
@@ -9904,8 +9958,11 @@
       <c r="AA114" s="9">
         <v>55.999466701546275</v>
       </c>
-    </row>
-    <row r="115" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB114" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="115" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>16</v>
       </c>
@@ -9982,7 +10039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>20</v>
       </c>
@@ -10059,7 +10116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>24</v>
       </c>
@@ -10136,7 +10193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>28</v>
       </c>
@@ -10213,7 +10270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>32</v>
       </c>
@@ -10290,7 +10347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>36</v>
       </c>
@@ -10367,7 +10424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>55</v>
       </c>
@@ -10450,8 +10507,11 @@
       <c r="AA121" s="9">
         <v>52.104653895086663</v>
       </c>
-    </row>
-    <row r="122" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB121" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>67</v>
       </c>
@@ -10528,7 +10588,7 @@
         <v>14.254100000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>77</v>
       </c>
@@ -10605,7 +10665,7 @@
         <v>13.208599999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>87</v>
       </c>
@@ -10682,7 +10742,7 @@
         <v>11.1829</v>
       </c>
     </row>
-    <row r="125" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>97</v>
       </c>
@@ -10759,7 +10819,7 @@
         <v>9.1695000000000011</v>
       </c>
     </row>
-    <row r="126" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>107</v>
       </c>
@@ -10836,7 +10896,7 @@
         <v>8.557599999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>117</v>
       </c>
@@ -10913,7 +10973,7 @@
         <v>8.8149999999999995</v>
       </c>
     </row>
-    <row r="128" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>57</v>
       </c>
@@ -10996,8 +11056,11 @@
       <c r="AA128" s="9">
         <v>60.057395161179436</v>
       </c>
-    </row>
-    <row r="129" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB128" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>68</v>
       </c>
@@ -11074,7 +11137,7 @@
         <v>19.708800000000004</v>
       </c>
     </row>
-    <row r="130" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>78</v>
       </c>
@@ -11151,7 +11214,7 @@
         <v>19.850200000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>88</v>
       </c>
@@ -11228,7 +11291,7 @@
         <v>19.947099999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>98</v>
       </c>
@@ -11305,7 +11368,7 @@
         <v>20.203799999999998</v>
       </c>
     </row>
-    <row r="133" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>108</v>
       </c>
@@ -11382,7 +11445,7 @@
         <v>20.465299999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>118</v>
       </c>
@@ -11459,7 +11522,7 @@
         <v>20.934400000000004</v>
       </c>
     </row>
-    <row r="135" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>12</v>
       </c>
@@ -11542,8 +11605,11 @@
       <c r="AA135" s="9">
         <v>44.970689041346482</v>
       </c>
-    </row>
-    <row r="136" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB135" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="136" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>17</v>
       </c>
@@ -11620,7 +11686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>21</v>
       </c>
@@ -11697,7 +11763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>25</v>
       </c>
@@ -11774,7 +11840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>29</v>
       </c>
@@ -11851,7 +11917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>33</v>
       </c>
@@ -11928,7 +11994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>37</v>
       </c>

</xml_diff>